<commit_message>
Revert "Update Checklist & Game logic"
This reverts commit 0fd1ddea0c88d8f91e631509046adaeb8c6795ad.
</commit_message>
<xml_diff>
--- a/Docs/UniBOOM_GanttDetail.xlsx
+++ b/Docs/UniBOOM_GanttDetail.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="46">
   <si>
     <t>测试</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -30,6 +30,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>赛博风场景模型</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>道具逻辑</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -42,14 +46,38 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>Dark Unitychan</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UI逻辑</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>音乐素材收集</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>素材收集</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>RPG风场景</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>工厂风场景</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>演出效果</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>演出效果</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>L.M</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -62,6 +90,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>StevenChangZH</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>地图自动生成</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -116,91 +148,55 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>整理</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>整理</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>赛博风怪物贴图</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>场景控制逻辑</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>RPG风怪物贴图</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>RPG风怪物模型</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>RPG风场景贴图</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>RPG风场景模型</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>工厂风怪物贴图</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>工场贴</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>工厂风场景贴图</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>地图自动生成</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>UI设计</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>RPG怪模</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>RPG怪模</t>
+    <t>工厂风场景模型</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>工厂风怪物模型</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>工厂场景模型</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>UI逻辑</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>UI逻辑</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>场景控制逻辑</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>音乐素材收集</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>RPG风场景</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>工厂风场景</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>演出效果</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>演出效果</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>杂项</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>杂项</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>StevenChang</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -368,7 +364,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -390,13 +386,43 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -405,44 +431,8 @@
     <xf numFmtId="176" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -747,23 +737,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AM5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AI10" sqref="AI10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="13" customWidth="1"/>
+    <col min="1" max="1" width="16" customWidth="1"/>
     <col min="7" max="8" width="9" style="4"/>
     <col min="14" max="15" width="9" style="4"/>
     <col min="16" max="17" width="9" customWidth="1"/>
     <col min="21" max="22" width="9" style="4"/>
-    <col min="27" max="27" width="9" customWidth="1"/>
     <col min="28" max="29" width="9" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:39">
-      <c r="A1" s="24"/>
       <c r="B1" s="1">
         <v>42128</v>
       </c>
@@ -818,7 +806,7 @@
       <c r="S1" s="1">
         <v>42145</v>
       </c>
-      <c r="T1" s="11">
+      <c r="T1" s="21">
         <v>42146</v>
       </c>
       <c r="U1" s="3">
@@ -880,288 +868,289 @@
       </c>
     </row>
     <row r="2" spans="1:39">
-      <c r="A2" s="24" t="s">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="11"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="10"/>
+      <c r="I2" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="K2" s="8"/>
+      <c r="L2" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="M2" s="11"/>
+      <c r="P2" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q2" s="10"/>
+      <c r="R2" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="S2" s="14"/>
+      <c r="T2" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="W2" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="X2" s="10"/>
+      <c r="Y2" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="20"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="F2" s="16"/>
-      <c r="I2" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="J2" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="K2" s="21"/>
-      <c r="L2" s="19" t="s">
+      <c r="Z2" s="11"/>
+      <c r="AA2" s="10"/>
+      <c r="AD2" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AE2" s="11"/>
+      <c r="AF2" s="10"/>
+      <c r="AG2" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="M2" s="20"/>
-      <c r="P2" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q2" s="21"/>
-      <c r="R2" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="S2" s="20"/>
-      <c r="T2" s="21"/>
-      <c r="W2" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="X2" s="20"/>
-      <c r="Y2" s="21"/>
-      <c r="Z2" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="AA2" s="16"/>
-      <c r="AD2" s="19" t="s">
-        <v>41</v>
-      </c>
-      <c r="AE2" s="21"/>
-      <c r="AF2" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="AG2" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="AH2" s="18"/>
-      <c r="AI2" s="12" t="s">
+      <c r="AH2" s="19"/>
+      <c r="AI2" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="AJ2" s="12"/>
-      <c r="AK2" s="12"/>
-      <c r="AL2" s="12"/>
-      <c r="AM2" s="13"/>
+      <c r="AJ2" s="16"/>
+      <c r="AK2" s="16"/>
+      <c r="AL2" s="16"/>
+      <c r="AM2" s="17"/>
     </row>
     <row r="3" spans="1:39">
-      <c r="A3" s="24" t="s">
-        <v>46</v>
-      </c>
-      <c r="B3" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" s="21"/>
-      <c r="D3" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="20"/>
-      <c r="F3" s="21"/>
-      <c r="I3" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="J3" s="21"/>
-      <c r="K3" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="L3" s="20"/>
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="10"/>
+      <c r="D3" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="11"/>
+      <c r="F3" s="10"/>
+      <c r="I3" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="J3" s="10"/>
+      <c r="K3" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="L3" s="11"/>
       <c r="M3" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="P3" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q3" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="R3" s="21"/>
-      <c r="S3" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="T3" s="21"/>
-      <c r="W3" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="X3" s="20"/>
-      <c r="Y3" s="21"/>
-      <c r="Z3" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="AA3" s="21"/>
-      <c r="AD3" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="AE3" s="20"/>
-      <c r="AF3" s="21"/>
-      <c r="AG3" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="AH3" s="18"/>
-      <c r="AI3" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="P3" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q3" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="R3" s="10"/>
+      <c r="S3" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="T3" s="17"/>
+      <c r="W3" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="X3" s="10"/>
+      <c r="Y3" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z3" s="11"/>
+      <c r="AA3" s="10"/>
+      <c r="AD3" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="AE3" s="11"/>
+      <c r="AF3" s="10"/>
+      <c r="AG3" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="AH3" s="19"/>
+      <c r="AI3" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="AJ3" s="12"/>
-      <c r="AK3" s="12"/>
-      <c r="AL3" s="12"/>
-      <c r="AM3" s="13"/>
+      <c r="AJ3" s="16"/>
+      <c r="AK3" s="16"/>
+      <c r="AL3" s="16"/>
+      <c r="AM3" s="17"/>
     </row>
     <row r="4" spans="1:39">
-      <c r="A4" s="24" t="s">
-        <v>9</v>
+      <c r="A4" t="s">
+        <v>16</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="21"/>
-      <c r="E4" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="F4" s="16"/>
-      <c r="I4" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="J4" s="17"/>
-      <c r="K4" s="17"/>
-      <c r="L4" s="17"/>
-      <c r="M4" s="16"/>
-      <c r="P4" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="Q4" s="16"/>
-      <c r="R4" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="S4" s="17"/>
-      <c r="T4" s="16"/>
-      <c r="W4" s="15" t="s">
+      <c r="D4" s="10"/>
+      <c r="E4" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="F4" s="8"/>
+      <c r="I4" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="X4" s="17"/>
-      <c r="Y4" s="15" t="s">
+      <c r="J4" s="14"/>
+      <c r="K4" s="8"/>
+      <c r="L4" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="M4" s="8"/>
+      <c r="P4" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="Z4" s="16"/>
+      <c r="Q4" s="14"/>
+      <c r="R4" s="8"/>
+      <c r="S4" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="T4" s="8"/>
+      <c r="W4" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="X4" s="14"/>
+      <c r="Y4" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z4" s="8"/>
       <c r="AA4" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="AD4" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="AE4" s="16"/>
-      <c r="AF4" s="14" t="s">
+      <c r="AD4" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="AE4" s="14"/>
+      <c r="AF4" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AG4" s="8"/>
+      <c r="AI4" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="AG4" s="12"/>
-      <c r="AH4" s="12"/>
-      <c r="AI4" s="12"/>
-      <c r="AJ4" s="12"/>
-      <c r="AK4" s="12"/>
-      <c r="AL4" s="12"/>
-      <c r="AM4" s="13"/>
+      <c r="AJ4" s="16"/>
+      <c r="AK4" s="16"/>
+      <c r="AL4" s="16"/>
+      <c r="AM4" s="17"/>
     </row>
     <row r="5" spans="1:39">
-      <c r="A5" s="24" t="s">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="16"/>
-      <c r="D5" s="15" t="s">
+      <c r="C5" s="8"/>
+      <c r="D5" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="16"/>
-      <c r="F5" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="I5" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="J5" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="K5" s="16"/>
-      <c r="L5" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="M5" s="16"/>
-      <c r="P5" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q5" s="16"/>
-      <c r="R5" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="S5" s="17"/>
-      <c r="T5" s="16"/>
-      <c r="W5" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="X5" s="16"/>
-      <c r="Y5" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="Z5" s="17"/>
-      <c r="AA5" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="AD5" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="AE5" s="16"/>
-      <c r="AF5" s="14" t="s">
+      <c r="E5" s="14"/>
+      <c r="F5" s="8"/>
+      <c r="I5" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="J5" s="14"/>
+      <c r="K5" s="8"/>
+      <c r="L5" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="M5" s="8"/>
+      <c r="P5" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q5" s="8"/>
+      <c r="R5" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="S5" s="14"/>
+      <c r="T5" s="8"/>
+      <c r="W5" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="X5" s="8"/>
+      <c r="Y5" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="Z5" s="14"/>
+      <c r="AA5" s="8"/>
+      <c r="AD5" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AE5" s="8"/>
+      <c r="AF5" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="AG5" s="8"/>
+      <c r="AI5" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="AG5" s="12"/>
-      <c r="AH5" s="12"/>
-      <c r="AI5" s="12"/>
-      <c r="AJ5" s="12"/>
-      <c r="AK5" s="12"/>
-      <c r="AL5" s="12"/>
-      <c r="AM5" s="13"/>
+      <c r="AJ5" s="16"/>
+      <c r="AK5" s="16"/>
+      <c r="AL5" s="16"/>
+      <c r="AM5" s="17"/>
     </row>
   </sheetData>
-  <mergeCells count="41">
-    <mergeCell ref="W5:X5"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="I4:M4"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="R2:T2"/>
-    <mergeCell ref="W2:Y2"/>
-    <mergeCell ref="W3:Y3"/>
-    <mergeCell ref="P4:Q4"/>
-    <mergeCell ref="R4:T4"/>
-    <mergeCell ref="Y5:Z5"/>
+  <mergeCells count="44">
+    <mergeCell ref="AI3:AM3"/>
+    <mergeCell ref="AI4:AM4"/>
+    <mergeCell ref="AI5:AM5"/>
+    <mergeCell ref="Y4:Z4"/>
+    <mergeCell ref="Y5:AA5"/>
+    <mergeCell ref="AG2:AH2"/>
+    <mergeCell ref="AG3:AH3"/>
+    <mergeCell ref="AD2:AF2"/>
+    <mergeCell ref="AD3:AF3"/>
+    <mergeCell ref="AD4:AE4"/>
+    <mergeCell ref="AD5:AE5"/>
+    <mergeCell ref="AF4:AG4"/>
+    <mergeCell ref="AF5:AG5"/>
+    <mergeCell ref="S3:T3"/>
+    <mergeCell ref="S4:T4"/>
+    <mergeCell ref="Y3:AA3"/>
+    <mergeCell ref="W4:X4"/>
+    <mergeCell ref="AI2:AM2"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="I3:J3"/>
     <mergeCell ref="L2:M2"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="P2:Q2"/>
     <mergeCell ref="Q3:R3"/>
+    <mergeCell ref="I5:K5"/>
+    <mergeCell ref="L4:M4"/>
+    <mergeCell ref="B5:C5"/>
     <mergeCell ref="K3:L3"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="C4:D4"/>
     <mergeCell ref="J2:K2"/>
+    <mergeCell ref="I4:K4"/>
     <mergeCell ref="L5:M5"/>
+    <mergeCell ref="W3:X3"/>
     <mergeCell ref="P5:Q5"/>
     <mergeCell ref="R5:T5"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="D3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="S3:T3"/>
-    <mergeCell ref="W4:X4"/>
-    <mergeCell ref="AI2:AM2"/>
-    <mergeCell ref="Z2:AA2"/>
-    <mergeCell ref="Z3:AA3"/>
-    <mergeCell ref="AD2:AE2"/>
-    <mergeCell ref="AF4:AM4"/>
-    <mergeCell ref="AG2:AH2"/>
-    <mergeCell ref="AG3:AH3"/>
-    <mergeCell ref="AD3:AF3"/>
-    <mergeCell ref="AD4:AE4"/>
-    <mergeCell ref="AI3:AM3"/>
-    <mergeCell ref="Y4:Z4"/>
-    <mergeCell ref="AD5:AE5"/>
-    <mergeCell ref="AF5:AM5"/>
+    <mergeCell ref="Y2:AA2"/>
+    <mergeCell ref="W5:X5"/>
+    <mergeCell ref="W2:X2"/>
+    <mergeCell ref="R2:S2"/>
+    <mergeCell ref="P4:R4"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Revert "Revert "Update Checklist & Game logic""
This reverts commit ec61716bc6036c9ccecd1c3b63a0d97346c1c25e.
</commit_message>
<xml_diff>
--- a/Docs/UniBOOM_GanttDetail.xlsx
+++ b/Docs/UniBOOM_GanttDetail.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="47">
   <si>
     <t>测试</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -30,10 +30,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>赛博风场景模型</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>道具逻辑</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -46,7 +42,121 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Dark Unitychan</t>
+    <t>素材收集</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>演出效果</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>L.M</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ScottFoH</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BigTree</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>地图自动生成</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CSV读取</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>高级敌人逻辑及AI</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>高AI</t>
+  </si>
+  <si>
+    <t>高AI</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>熟悉项目</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>熟悉项目</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>赛博风场景贴图</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BOSS逻辑及AI</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UI要素制作</t>
+  </si>
+  <si>
+    <t>UI设计</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UI要素制作</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UI要素制作</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BOSS逻辑及AI</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>赛博风怪物贴图</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RPG风怪物贴图</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RPG风场景贴图</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>工厂风怪物贴图</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>工厂风场景贴图</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>地图自动生成</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UI设计</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RPG怪模</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RPG怪模</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>工厂风怪物模型</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>工厂场景模型</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -54,14 +164,18 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>UI逻辑</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>场景控制逻辑</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>音乐素材收集</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>素材收集</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>RPG风场景</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -78,125 +192,15 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>L.M</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ScottFoH</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BigTree</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>StevenChangZH</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>地图自动生成</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CSV读取</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>高级敌人逻辑及AI</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>高AI</t>
-  </si>
-  <si>
-    <t>高AI</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>熟悉项目</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>熟悉项目</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>赛博风场景贴图</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BOSS逻辑及AI</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>UI要素制作</t>
-  </si>
-  <si>
-    <t>UI设计</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>UI要素制作</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>UI要素制作</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BOSS逻辑及AI</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>整理</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>整理</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>赛博风怪物贴图</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>场景控制逻辑</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>RPG风怪物贴图</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>RPG风怪物模型</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>RPG风场景贴图</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>RPG风场景模型</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>工厂风怪物贴图</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>工场贴</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>工厂风场景贴图</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>工厂风场景模型</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>工厂风怪物模型</t>
+    <t>杂项</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>杂项</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>StevenChang</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -364,7 +368,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -386,43 +390,13 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -431,8 +405,44 @@
     <xf numFmtId="176" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -737,21 +747,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AM5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AI10" sqref="AI10"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="1" max="1" width="13" customWidth="1"/>
     <col min="7" max="8" width="9" style="4"/>
     <col min="14" max="15" width="9" style="4"/>
     <col min="16" max="17" width="9" customWidth="1"/>
     <col min="21" max="22" width="9" style="4"/>
+    <col min="27" max="27" width="9" customWidth="1"/>
     <col min="28" max="29" width="9" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:39">
+      <c r="A1" s="24"/>
       <c r="B1" s="1">
         <v>42128</v>
       </c>
@@ -806,7 +818,7 @@
       <c r="S1" s="1">
         <v>42145</v>
       </c>
-      <c r="T1" s="21">
+      <c r="T1" s="11">
         <v>42146</v>
       </c>
       <c r="U1" s="3">
@@ -868,289 +880,288 @@
       </c>
     </row>
     <row r="2" spans="1:39">
-      <c r="A2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" s="9" t="s">
+      <c r="A2" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="9" t="s">
+      <c r="C2" s="20"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" s="16"/>
+      <c r="I2" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="J2" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="K2" s="21"/>
+      <c r="L2" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="M2" s="20"/>
+      <c r="P2" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="10"/>
-      <c r="I2" s="20" t="s">
-        <v>4</v>
-      </c>
-      <c r="J2" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="K2" s="8"/>
-      <c r="L2" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="M2" s="11"/>
-      <c r="P2" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q2" s="10"/>
-      <c r="R2" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="S2" s="14"/>
-      <c r="T2" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="W2" s="11" t="s">
+      <c r="Q2" s="21"/>
+      <c r="R2" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="X2" s="10"/>
-      <c r="Y2" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="Z2" s="11"/>
-      <c r="AA2" s="10"/>
-      <c r="AD2" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="AE2" s="11"/>
-      <c r="AF2" s="10"/>
-      <c r="AG2" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="AH2" s="19"/>
-      <c r="AI2" s="16" t="s">
+      <c r="S2" s="20"/>
+      <c r="T2" s="21"/>
+      <c r="W2" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="X2" s="20"/>
+      <c r="Y2" s="21"/>
+      <c r="Z2" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="AA2" s="16"/>
+      <c r="AD2" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="AE2" s="21"/>
+      <c r="AF2" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="AG2" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="AH2" s="18"/>
+      <c r="AI2" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="AJ2" s="16"/>
-      <c r="AK2" s="16"/>
-      <c r="AL2" s="16"/>
-      <c r="AM2" s="17"/>
+      <c r="AJ2" s="12"/>
+      <c r="AK2" s="12"/>
+      <c r="AL2" s="12"/>
+      <c r="AM2" s="13"/>
     </row>
     <row r="3" spans="1:39">
-      <c r="A3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" s="9" t="s">
+      <c r="A3" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="21"/>
+      <c r="D3" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="20"/>
+      <c r="F3" s="21"/>
+      <c r="I3" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="J3" s="21"/>
+      <c r="K3" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="L3" s="20"/>
+      <c r="M3" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="P3" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q3" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="10"/>
-      <c r="D3" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" s="11"/>
-      <c r="F3" s="10"/>
-      <c r="I3" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="J3" s="10"/>
-      <c r="K3" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="L3" s="11"/>
-      <c r="M3" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="P3" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q3" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="R3" s="10"/>
-      <c r="S3" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="T3" s="17"/>
-      <c r="W3" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="X3" s="10"/>
-      <c r="Y3" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="Z3" s="11"/>
-      <c r="AA3" s="10"/>
-      <c r="AD3" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="AE3" s="11"/>
-      <c r="AF3" s="10"/>
-      <c r="AG3" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="AH3" s="19"/>
-      <c r="AI3" s="16" t="s">
+      <c r="R3" s="21"/>
+      <c r="S3" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="T3" s="21"/>
+      <c r="W3" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="X3" s="20"/>
+      <c r="Y3" s="21"/>
+      <c r="Z3" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA3" s="21"/>
+      <c r="AD3" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="AE3" s="20"/>
+      <c r="AF3" s="21"/>
+      <c r="AG3" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="AH3" s="18"/>
+      <c r="AI3" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="AJ3" s="16"/>
-      <c r="AK3" s="16"/>
-      <c r="AL3" s="16"/>
-      <c r="AM3" s="17"/>
+      <c r="AJ3" s="12"/>
+      <c r="AK3" s="12"/>
+      <c r="AL3" s="12"/>
+      <c r="AM3" s="13"/>
     </row>
     <row r="4" spans="1:39">
-      <c r="A4" t="s">
-        <v>16</v>
+      <c r="A4" s="24" t="s">
+        <v>9</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="21"/>
+      <c r="E4" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="16"/>
+      <c r="I4" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="J4" s="17"/>
+      <c r="K4" s="17"/>
+      <c r="L4" s="17"/>
+      <c r="M4" s="16"/>
+      <c r="P4" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q4" s="16"/>
+      <c r="R4" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" s="10"/>
-      <c r="E4" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="F4" s="8"/>
-      <c r="I4" s="7" t="s">
+      <c r="S4" s="17"/>
+      <c r="T4" s="16"/>
+      <c r="W4" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="J4" s="14"/>
-      <c r="K4" s="8"/>
-      <c r="L4" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="M4" s="8"/>
-      <c r="P4" s="7" t="s">
+      <c r="X4" s="17"/>
+      <c r="Y4" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="Q4" s="14"/>
-      <c r="R4" s="8"/>
-      <c r="S4" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="T4" s="8"/>
-      <c r="W4" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="X4" s="14"/>
-      <c r="Y4" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="Z4" s="8"/>
+      <c r="Z4" s="16"/>
       <c r="AA4" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="AD4" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="AE4" s="14"/>
-      <c r="AF4" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="AG4" s="8"/>
-      <c r="AI4" s="15" t="s">
+      <c r="AD4" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="AE4" s="16"/>
+      <c r="AF4" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="AJ4" s="16"/>
-      <c r="AK4" s="16"/>
-      <c r="AL4" s="16"/>
-      <c r="AM4" s="17"/>
+      <c r="AG4" s="12"/>
+      <c r="AH4" s="12"/>
+      <c r="AI4" s="12"/>
+      <c r="AJ4" s="12"/>
+      <c r="AK4" s="12"/>
+      <c r="AL4" s="12"/>
+      <c r="AM4" s="13"/>
     </row>
     <row r="5" spans="1:39">
-      <c r="A5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" s="7" t="s">
+      <c r="A5" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="8"/>
-      <c r="D5" s="7" t="s">
+      <c r="B5" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="16"/>
+      <c r="D5" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="14"/>
-      <c r="F5" s="8"/>
-      <c r="I5" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="J5" s="14"/>
-      <c r="K5" s="8"/>
-      <c r="L5" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="M5" s="8"/>
-      <c r="P5" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q5" s="8"/>
-      <c r="R5" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="S5" s="14"/>
-      <c r="T5" s="8"/>
-      <c r="W5" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="X5" s="8"/>
-      <c r="Y5" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="Z5" s="14"/>
-      <c r="AA5" s="8"/>
-      <c r="AD5" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="AE5" s="8"/>
-      <c r="AF5" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="AG5" s="8"/>
-      <c r="AI5" s="15" t="s">
+      <c r="E5" s="16"/>
+      <c r="F5" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="J5" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="K5" s="16"/>
+      <c r="L5" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="M5" s="16"/>
+      <c r="P5" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q5" s="16"/>
+      <c r="R5" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="S5" s="17"/>
+      <c r="T5" s="16"/>
+      <c r="W5" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="X5" s="16"/>
+      <c r="Y5" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z5" s="17"/>
+      <c r="AA5" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="AD5" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="AE5" s="16"/>
+      <c r="AF5" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="AJ5" s="16"/>
-      <c r="AK5" s="16"/>
-      <c r="AL5" s="16"/>
-      <c r="AM5" s="17"/>
+      <c r="AG5" s="12"/>
+      <c r="AH5" s="12"/>
+      <c r="AI5" s="12"/>
+      <c r="AJ5" s="12"/>
+      <c r="AK5" s="12"/>
+      <c r="AL5" s="12"/>
+      <c r="AM5" s="13"/>
     </row>
   </sheetData>
-  <mergeCells count="44">
-    <mergeCell ref="AI3:AM3"/>
-    <mergeCell ref="AI4:AM4"/>
-    <mergeCell ref="AI5:AM5"/>
-    <mergeCell ref="Y4:Z4"/>
-    <mergeCell ref="Y5:AA5"/>
-    <mergeCell ref="AG2:AH2"/>
-    <mergeCell ref="AG3:AH3"/>
-    <mergeCell ref="AD2:AF2"/>
-    <mergeCell ref="AD3:AF3"/>
-    <mergeCell ref="AD4:AE4"/>
-    <mergeCell ref="AD5:AE5"/>
-    <mergeCell ref="AF4:AG4"/>
-    <mergeCell ref="AF5:AG5"/>
-    <mergeCell ref="S3:T3"/>
-    <mergeCell ref="S4:T4"/>
-    <mergeCell ref="Y3:AA3"/>
-    <mergeCell ref="W4:X4"/>
-    <mergeCell ref="AI2:AM2"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="D5:F5"/>
-    <mergeCell ref="D3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="I3:J3"/>
+  <mergeCells count="41">
+    <mergeCell ref="W5:X5"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="I4:M4"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="R2:T2"/>
+    <mergeCell ref="W2:Y2"/>
+    <mergeCell ref="W3:Y3"/>
+    <mergeCell ref="P4:Q4"/>
+    <mergeCell ref="R4:T4"/>
+    <mergeCell ref="Y5:Z5"/>
     <mergeCell ref="L2:M2"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="P2:Q2"/>
     <mergeCell ref="Q3:R3"/>
-    <mergeCell ref="I5:K5"/>
-    <mergeCell ref="L4:M4"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="P5:Q5"/>
+    <mergeCell ref="R5:T5"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="I3:J3"/>
     <mergeCell ref="B5:C5"/>
-    <mergeCell ref="K3:L3"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="C4:D4"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="I4:K4"/>
-    <mergeCell ref="L5:M5"/>
-    <mergeCell ref="W3:X3"/>
-    <mergeCell ref="P5:Q5"/>
-    <mergeCell ref="R5:T5"/>
-    <mergeCell ref="Y2:AA2"/>
-    <mergeCell ref="W5:X5"/>
-    <mergeCell ref="W2:X2"/>
-    <mergeCell ref="R2:S2"/>
-    <mergeCell ref="P4:R4"/>
+    <mergeCell ref="S3:T3"/>
+    <mergeCell ref="W4:X4"/>
+    <mergeCell ref="AI2:AM2"/>
+    <mergeCell ref="Z2:AA2"/>
+    <mergeCell ref="Z3:AA3"/>
+    <mergeCell ref="AD2:AE2"/>
+    <mergeCell ref="AF4:AM4"/>
+    <mergeCell ref="AG2:AH2"/>
+    <mergeCell ref="AG3:AH3"/>
+    <mergeCell ref="AD3:AF3"/>
+    <mergeCell ref="AD4:AE4"/>
+    <mergeCell ref="AI3:AM3"/>
+    <mergeCell ref="Y4:Z4"/>
+    <mergeCell ref="AD5:AE5"/>
+    <mergeCell ref="AF5:AM5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>